<commit_message>
Update template metadata spreadsheet
</commit_message>
<xml_diff>
--- a/examples/processing_metadata_template.xlsx
+++ b/examples/processing_metadata_template.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abarrera/workspace/ggr-cwl-ipynb-gen/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aeb84/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D758F8-5465-0A46-B776-A07D35947F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="14640" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="4" r:id="rId2"/>
+    <sheet name="options" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$75</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="68">
   <si>
     <t>Sequencing core project</t>
   </si>
@@ -47,12 +50,6 @@
     <t>Library type</t>
   </si>
   <si>
-    <t>Sequencing core user</t>
-  </si>
-  <si>
-    <t>Sequencing core password</t>
-  </si>
-  <si>
     <t>SE</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Control</t>
   </si>
   <si>
-    <t>lab_4821</t>
-  </si>
-  <si>
     <t>Reddy_4821_180419A3</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>XXXXXXX</t>
-  </si>
-  <si>
     <t>with ercc spike-in</t>
   </si>
   <si>
@@ -150,13 +141,149 @@
   </si>
   <si>
     <t>UMIs</t>
+  </si>
+  <si>
+    <t>unstranded</t>
+  </si>
+  <si>
+    <t>stranded</t>
+  </si>
+  <si>
+    <t>hg19</t>
+  </si>
+  <si>
+    <t>mm10</t>
+  </si>
+  <si>
+    <t>mm9</t>
+  </si>
+  <si>
+    <t>danrer10</t>
+  </si>
+  <si>
+    <t>Binary columns</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project name. Will be used as the project descriptor and to create intermediate folders </t>
+  </si>
+  <si>
+    <t>Reddy_4562_210911A6</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sample name as identified in the files coming directly from the sequencing core or instrument. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Do not inlcude the sample ID and any trailing characters </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(e.g. _S1_001_L001_fastq.gz)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Desired sample name, including some special chacaters </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>but excluding whitespaces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>. It will be used as the unique sample basename.</t>
+    </r>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>Library sequencing modality</t>
+  </si>
+  <si>
+    <t>SE, PE</t>
+  </si>
+  <si>
+    <t>Reference genome to be used</t>
+  </si>
+  <si>
+    <t>hg38, hg19, mm10, mm9, danrer10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment type being processed </t>
+  </si>
+  <si>
+    <t>ChIP-seq, RNA-seq, STARR-seq, ATAC-seq</t>
+  </si>
+  <si>
+    <t>Experiments applicable</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Whether or not the experiment includes UMIs</t>
+  </si>
+  <si>
+    <t>yes, no</t>
+  </si>
+  <si>
+    <t>Sample "Name" of the input control sample. Please include the control sample as its own entry in the list (with the an empty Control column)</t>
+  </si>
+  <si>
+    <t>Any sample Name already added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depending on the type of protocol used, there might be information regarding the strand of RNA being transcribed (stranded) or not (unstranded). Additionally, most protocols will actually generate reads from the reverse complement of the originating mRNA transcript (revstranded). </t>
+  </si>
+  <si>
+    <t>unstranded, stranded, revstranded</t>
+  </si>
+  <si>
+    <t>Whether or not the blacklist with poor mappability rates (from ENCODE)</t>
+  </si>
+  <si>
+    <t>Whether or not ERCC spike-ins were used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,6 +320,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,7 +374,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -210,6 +382,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -363,10 +544,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="150">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -525,6 +732,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -851,322 +1061,630 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="10.83203125" style="1"/>
-    <col min="20" max="20" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="J6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{164DCB9F-45B0-E144-84AC-31D5CAA37ABD}">
+          <x14:formula1>
+            <xm:f>options!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BF262A3B-FDAB-1B40-BA9B-08773AD489B8}">
+          <x14:formula1>
+            <xm:f>options!$B$2:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{605C814A-4771-D745-B0FD-0F8C12C25D16}">
+          <x14:formula1>
+            <xm:f>options!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D245042-8D59-3441-9D61-3E5A51FE700F}">
+          <x14:formula1>
+            <xm:f>options!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G9 J2:K9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{910DE98F-2756-2E48-8532-F28936F2EBF3}">
+          <x14:formula1>
+            <xm:f>options!$E$2:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B81E10-C836-DA48-899D-9330EF41A240}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="51" style="7" customWidth="1"/>
+    <col min="4" max="4" width="36.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="38.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="44" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="66" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="66" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="22" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="22" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="22" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="22" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="66" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="110" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="44" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="22" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349F05D4-33D1-3645-AF41-CE066AD8C167}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>